<commit_message>
fixed raw payroll period
</commit_message>
<xml_diff>
--- a/Generated file/Raw.xlsx
+++ b/Generated file/Raw.xlsx
@@ -727,7 +727,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -895,7 +895,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -923,7 +923,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>04.22 - 05.05</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1623,7 +1623,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1707,7 +1707,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1847,7 +1847,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1875,7 +1875,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2015,7 +2015,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2043,7 +2043,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2127,7 +2127,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>04.23 - 05.06</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2183,7 +2183,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2239,7 +2239,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2295,7 +2295,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2407,7 +2407,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2519,7 +2519,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -2575,7 +2575,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -2631,7 +2631,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -2715,7 +2715,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -2743,7 +2743,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -2771,7 +2771,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -2883,7 +2883,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -2911,7 +2911,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>04.24 - 05.07</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -3079,7 +3079,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -3107,7 +3107,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -3191,7 +3191,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -3219,7 +3219,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -3247,7 +3247,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -3275,7 +3275,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -3303,7 +3303,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -3387,7 +3387,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -3471,7 +3471,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -3499,7 +3499,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -3611,7 +3611,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -3639,7 +3639,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -3667,7 +3667,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -3695,7 +3695,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -3723,7 +3723,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -3779,7 +3779,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -3807,7 +3807,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>04.25 - 05.08</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -3919,7 +3919,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -3947,7 +3947,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -3975,7 +3975,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -4003,7 +4003,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -4031,7 +4031,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -4059,7 +4059,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -4087,7 +4087,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -4115,7 +4115,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -4171,7 +4171,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -4227,7 +4227,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -4311,7 +4311,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -4367,7 +4367,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -4395,7 +4395,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -4423,7 +4423,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -4451,7 +4451,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -4479,7 +4479,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -4535,7 +4535,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -4563,7 +4563,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -4619,7 +4619,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -4647,7 +4647,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -4675,7 +4675,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -4703,7 +4703,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>04.26 - 05.09</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -4731,7 +4731,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -4759,7 +4759,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -4787,7 +4787,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -4815,7 +4815,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -4843,7 +4843,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -4899,7 +4899,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -4927,7 +4927,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -4955,7 +4955,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -4983,7 +4983,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -5011,7 +5011,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -5039,7 +5039,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -5067,7 +5067,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -5123,7 +5123,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>04.27 - 05.10</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -5151,7 +5151,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>04.28 - 05.11</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -5179,7 +5179,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>04.28 - 05.11</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -5207,7 +5207,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>04.28 - 05.11</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>04.28 - 05.11</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>04.28 - 05.11</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5291,7 +5291,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>04.28 - 05.11</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5319,7 +5319,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>04.28 - 05.11</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -5347,7 +5347,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -5375,7 +5375,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -5403,7 +5403,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5431,7 +5431,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5459,7 +5459,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -5487,7 +5487,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -5515,7 +5515,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -5571,7 +5571,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -5599,7 +5599,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -5627,7 +5627,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -5655,7 +5655,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -5683,7 +5683,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -5739,7 +5739,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -5767,7 +5767,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -5795,7 +5795,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -5823,7 +5823,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -5851,7 +5851,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -5879,7 +5879,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -5907,7 +5907,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -5935,7 +5935,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -5963,7 +5963,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -5991,7 +5991,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6019,7 +6019,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -6047,7 +6047,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -6075,7 +6075,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6103,7 +6103,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6131,7 +6131,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>04.29 - 05.12</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6159,7 +6159,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -6187,7 +6187,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -6215,7 +6215,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6243,7 +6243,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6271,7 +6271,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6299,7 +6299,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6327,7 +6327,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6355,7 +6355,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6383,7 +6383,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -6411,7 +6411,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -6439,7 +6439,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -6467,7 +6467,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -6495,7 +6495,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -6523,7 +6523,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -6551,7 +6551,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -6579,7 +6579,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -6607,7 +6607,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -6635,7 +6635,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -6663,7 +6663,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -6691,7 +6691,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -6719,7 +6719,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -6747,7 +6747,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -6775,7 +6775,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -6831,7 +6831,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -6859,7 +6859,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -6887,7 +6887,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -6915,7 +6915,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -6943,7 +6943,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -6971,7 +6971,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>04.30 - 05.13</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -6999,7 +6999,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7027,7 +7027,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7055,7 +7055,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7083,7 +7083,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7139,7 +7139,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -7167,7 +7167,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7195,7 +7195,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7251,7 +7251,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -7279,7 +7279,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -7307,7 +7307,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -7335,7 +7335,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -7363,7 +7363,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -7391,7 +7391,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -7419,7 +7419,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -7447,7 +7447,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -7475,7 +7475,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -7503,7 +7503,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -7531,7 +7531,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -7559,7 +7559,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -7587,7 +7587,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -7615,7 +7615,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -7643,7 +7643,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -7671,7 +7671,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -7699,7 +7699,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -7727,7 +7727,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -7755,7 +7755,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -7783,7 +7783,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -7811,7 +7811,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -7839,7 +7839,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>05.01 - 05.14</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -7867,7 +7867,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -7895,7 +7895,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -7923,7 +7923,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -7951,7 +7951,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -7979,7 +7979,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -8007,7 +8007,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8035,7 +8035,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8063,7 +8063,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -8091,7 +8091,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -8119,7 +8119,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -8147,7 +8147,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -8175,7 +8175,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -8203,7 +8203,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -8231,7 +8231,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -8259,7 +8259,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -8287,7 +8287,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -8315,7 +8315,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -8343,7 +8343,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -8371,7 +8371,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -8399,7 +8399,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -8427,7 +8427,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -8455,7 +8455,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -8483,7 +8483,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -8511,7 +8511,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -8539,7 +8539,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -8567,7 +8567,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -8595,7 +8595,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -8623,7 +8623,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -8651,7 +8651,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -8679,7 +8679,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>05.02 - 05.15</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -8707,7 +8707,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -8735,7 +8735,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -8763,7 +8763,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -8791,7 +8791,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -8819,7 +8819,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -8847,7 +8847,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -8875,7 +8875,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -8903,7 +8903,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -8931,7 +8931,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -8959,7 +8959,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -8987,7 +8987,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -9015,7 +9015,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -9043,7 +9043,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -9071,7 +9071,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -9099,7 +9099,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -9127,7 +9127,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -9155,7 +9155,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -9183,7 +9183,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -9239,7 +9239,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -9267,7 +9267,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -9295,7 +9295,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -9323,7 +9323,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -9351,7 +9351,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>05.03 - 05.16</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -9379,7 +9379,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -9407,7 +9407,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -9435,7 +9435,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -9463,7 +9463,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -9491,7 +9491,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -9519,7 +9519,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -9547,7 +9547,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -9575,7 +9575,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -9603,7 +9603,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -9631,7 +9631,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>05.04 - 05.17</t>
+          <t>04.21 - 05.04</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">

</xml_diff>